<commit_message>
add category to climb queries for OrientDB
</commit_message>
<xml_diff>
--- a/xlsx/vertices/climbs.xlsx
+++ b/xlsx/vertices/climbs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Documents\Dodo\M2\S2\DBMS\projet\graph\csv\xlsx\vertices\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Documents\Dodo\M2\S2\DBMS\projet\graph\data\xlsx\vertices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC36FD9B-A18D-44B3-AB9D-05B8F2C9221B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1FE0F18-0CC4-446E-B504-C078D7337A20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30045" yWindow="3165" windowWidth="28800" windowHeight="15435" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2869,10 +2869,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G64"/>
+    <sheetView topLeftCell="C34" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2892,12 +2892,12 @@
     <col min="13" max="13" width="63.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A2)=2,CHAR(34),""),climbs!A2,IF(TYPE(climbs!A2)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=1</v>
@@ -2926,8 +2926,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G2)=2,CHAR(34),""),climbs!G2,IF(TYPE(climbs!G2)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=7.1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H2)=2,CHAR(34),""),climbs!H2,IF(TYPE(climbs!H2)=2,CHAR(34),""))</f>
+        <v>CATEGORY="4"</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A3)=2,CHAR(34),""),climbs!A3,IF(TYPE(climbs!A3)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=2</v>
@@ -2956,8 +2960,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G3)=2,CHAR(34),""),climbs!G3,IF(TYPE(climbs!G3)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=6.8</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H3)=2,CHAR(34),""),climbs!H3,IF(TYPE(climbs!H3)=2,CHAR(34),""))</f>
+        <v>CATEGORY="3"</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A4)=2,CHAR(34),""),climbs!A4,IF(TYPE(climbs!A4)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=3</v>
@@ -2986,8 +2994,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G4)=2,CHAR(34),""),climbs!G4,IF(TYPE(climbs!G4)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=6.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H4)=2,CHAR(34),""),climbs!H4,IF(TYPE(climbs!H4)=2,CHAR(34),""))</f>
+        <v>CATEGORY="3"</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A5)=2,CHAR(34),""),climbs!A5,IF(TYPE(climbs!A5)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=4</v>
@@ -3016,8 +3028,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G5)=2,CHAR(34),""),climbs!G5,IF(TYPE(climbs!G5)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=6.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H5)=2,CHAR(34),""),climbs!H5,IF(TYPE(climbs!H5)=2,CHAR(34),""))</f>
+        <v>CATEGORY="4"</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A6)=2,CHAR(34),""),climbs!A6,IF(TYPE(climbs!A6)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=5</v>
@@ -3046,8 +3062,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G6)=2,CHAR(34),""),climbs!G6,IF(TYPE(climbs!G6)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=6.4</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H6)=2,CHAR(34),""),climbs!H6,IF(TYPE(climbs!H6)=2,CHAR(34),""))</f>
+        <v>CATEGORY="3"</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A7)=2,CHAR(34),""),climbs!A7,IF(TYPE(climbs!A7)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=6</v>
@@ -3076,8 +3096,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G7)=2,CHAR(34),""),climbs!G7,IF(TYPE(climbs!G7)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=8.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H7)=2,CHAR(34),""),climbs!H7,IF(TYPE(climbs!H7)=2,CHAR(34),""))</f>
+        <v>CATEGORY="3"</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A8)=2,CHAR(34),""),climbs!A8,IF(TYPE(climbs!A8)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=7</v>
@@ -3106,8 +3130,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G8)=2,CHAR(34),""),climbs!G8,IF(TYPE(climbs!G8)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=6.7</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H8)=2,CHAR(34),""),climbs!H8,IF(TYPE(climbs!H8)=2,CHAR(34),""))</f>
+        <v>CATEGORY="3"</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A9)=2,CHAR(34),""),climbs!A9,IF(TYPE(climbs!A9)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=8</v>
@@ -3136,8 +3164,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G9)=2,CHAR(34),""),climbs!G9,IF(TYPE(climbs!G9)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=7</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H9)=2,CHAR(34),""),climbs!H9,IF(TYPE(climbs!H9)=2,CHAR(34),""))</f>
+        <v>CATEGORY="2"</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A10)=2,CHAR(34),""),climbs!A10,IF(TYPE(climbs!A10)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=9</v>
@@ -3166,8 +3198,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G10)=2,CHAR(34),""),climbs!G10,IF(TYPE(climbs!G10)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=6.1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H10)=2,CHAR(34),""),climbs!H10,IF(TYPE(climbs!H10)=2,CHAR(34),""))</f>
+        <v>CATEGORY="3"</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A11)=2,CHAR(34),""),climbs!A11,IF(TYPE(climbs!A11)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=10</v>
@@ -3196,8 +3232,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G11)=2,CHAR(34),""),climbs!G11,IF(TYPE(climbs!G11)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=7.4</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H11)=2,CHAR(34),""),climbs!H11,IF(TYPE(climbs!H11)=2,CHAR(34),""))</f>
+        <v>CATEGORY="4"</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A12)=2,CHAR(34),""),climbs!A12,IF(TYPE(climbs!A12)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=11</v>
@@ -3226,8 +3266,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G12)=2,CHAR(34),""),climbs!G12,IF(TYPE(climbs!G12)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=9.1</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H12)=2,CHAR(34),""),climbs!H12,IF(TYPE(climbs!H12)=2,CHAR(34),""))</f>
+        <v>CATEGORY="3"</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A13)=2,CHAR(34),""),climbs!A13,IF(TYPE(climbs!A13)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=12</v>
@@ -3256,8 +3300,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G13)=2,CHAR(34),""),climbs!G13,IF(TYPE(climbs!G13)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=10.8</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H13)=2,CHAR(34),""),climbs!H13,IF(TYPE(climbs!H13)=2,CHAR(34),""))</f>
+        <v>CATEGORY="4"</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A14)=2,CHAR(34),""),climbs!A14,IF(TYPE(climbs!A14)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=13</v>
@@ -3286,8 +3334,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G14)=2,CHAR(34),""),climbs!G14,IF(TYPE(climbs!G14)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=6.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H14)=2,CHAR(34),""),climbs!H14,IF(TYPE(climbs!H14)=2,CHAR(34),""))</f>
+        <v>CATEGORY="4"</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A15)=2,CHAR(34),""),climbs!A15,IF(TYPE(climbs!A15)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=14</v>
@@ -3316,8 +3368,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G15)=2,CHAR(34),""),climbs!G15,IF(TYPE(climbs!G15)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=5.7</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H15)=2,CHAR(34),""),climbs!H15,IF(TYPE(climbs!H15)=2,CHAR(34),""))</f>
+        <v>CATEGORY="4"</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A16)=2,CHAR(34),""),climbs!A16,IF(TYPE(climbs!A16)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=15</v>
@@ -3346,8 +3402,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G16)=2,CHAR(34),""),climbs!G16,IF(TYPE(climbs!G16)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=6.2</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H16)=2,CHAR(34),""),climbs!H16,IF(TYPE(climbs!H16)=2,CHAR(34),""))</f>
+        <v>CATEGORY="4"</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A17)=2,CHAR(34),""),climbs!A17,IF(TYPE(climbs!A17)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=16</v>
@@ -3376,8 +3436,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G17)=2,CHAR(34),""),climbs!G17,IF(TYPE(climbs!G17)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=6.2</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H17)=2,CHAR(34),""),climbs!H17,IF(TYPE(climbs!H17)=2,CHAR(34),""))</f>
+        <v>CATEGORY="4"</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A18)=2,CHAR(34),""),climbs!A18,IF(TYPE(climbs!A18)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=17</v>
@@ -3406,8 +3470,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G18)=2,CHAR(34),""),climbs!G18,IF(TYPE(climbs!G18)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=5</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H18)=2,CHAR(34),""),climbs!H18,IF(TYPE(climbs!H18)=2,CHAR(34),""))</f>
+        <v>CATEGORY="4"</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A19)=2,CHAR(34),""),climbs!A19,IF(TYPE(climbs!A19)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=18</v>
@@ -3436,8 +3504,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G19)=2,CHAR(34),""),climbs!G19,IF(TYPE(climbs!G19)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=7.9</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H19)=2,CHAR(34),""),climbs!H19,IF(TYPE(climbs!H19)=2,CHAR(34),""))</f>
+        <v>CATEGORY="4"</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A20)=2,CHAR(34),""),climbs!A20,IF(TYPE(climbs!A20)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=19</v>
@@ -3466,8 +3538,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G20)=2,CHAR(34),""),climbs!G20,IF(TYPE(climbs!G20)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=6</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H20)=2,CHAR(34),""),climbs!H20,IF(TYPE(climbs!H20)=2,CHAR(34),""))</f>
+        <v>CATEGORY="2"</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A21)=2,CHAR(34),""),climbs!A21,IF(TYPE(climbs!A21)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=20</v>
@@ -3496,8 +3572,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G21)=2,CHAR(34),""),climbs!G21,IF(TYPE(climbs!G21)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=7.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H21)=2,CHAR(34),""),climbs!H21,IF(TYPE(climbs!H21)=2,CHAR(34),""))</f>
+        <v>CATEGORY="2"</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A22)=2,CHAR(34),""),climbs!A22,IF(TYPE(climbs!A22)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=21</v>
@@ -3526,8 +3606,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G22)=2,CHAR(34),""),climbs!G22,IF(TYPE(climbs!G22)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=10.3</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H22)=2,CHAR(34),""),climbs!H22,IF(TYPE(climbs!H22)=2,CHAR(34),""))</f>
+        <v>CATEGORY="3"</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A23)=2,CHAR(34),""),climbs!A23,IF(TYPE(climbs!A23)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=22</v>
@@ -3556,8 +3640,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G23)=2,CHAR(34),""),climbs!G23,IF(TYPE(climbs!G23)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=4.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H23)=2,CHAR(34),""),climbs!H23,IF(TYPE(climbs!H23)=2,CHAR(34),""))</f>
+        <v>CATEGORY="2"</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A24)=2,CHAR(34),""),climbs!A24,IF(TYPE(climbs!A24)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=23</v>
@@ -3586,8 +3674,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G24)=2,CHAR(34),""),climbs!G24,IF(TYPE(climbs!G24)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=4.1</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H24)=2,CHAR(34),""),climbs!H24,IF(TYPE(climbs!H24)=2,CHAR(34),""))</f>
+        <v>CATEGORY="3"</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A25)=2,CHAR(34),""),climbs!A25,IF(TYPE(climbs!A25)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=24</v>
@@ -3616,8 +3708,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G25)=2,CHAR(34),""),climbs!G25,IF(TYPE(climbs!G25)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=6.1</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H25)=2,CHAR(34),""),climbs!H25,IF(TYPE(climbs!H25)=2,CHAR(34),""))</f>
+        <v>CATEGORY="3"</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A26)=2,CHAR(34),""),climbs!A26,IF(TYPE(climbs!A26)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=25</v>
@@ -3646,8 +3742,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G26)=2,CHAR(34),""),climbs!G26,IF(TYPE(climbs!G26)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=7.9</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H26)=2,CHAR(34),""),climbs!H26,IF(TYPE(climbs!H26)=2,CHAR(34),""))</f>
+        <v>CATEGORY="2"</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A27)=2,CHAR(34),""),climbs!A27,IF(TYPE(climbs!A27)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=26</v>
@@ -3676,8 +3776,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G27)=2,CHAR(34),""),climbs!G27,IF(TYPE(climbs!G27)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=5.4</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H27)=2,CHAR(34),""),climbs!H27,IF(TYPE(climbs!H27)=2,CHAR(34),""))</f>
+        <v>CATEGORY="1"</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A28)=2,CHAR(34),""),climbs!A28,IF(TYPE(climbs!A28)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=27</v>
@@ -3706,8 +3810,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G28)=2,CHAR(34),""),climbs!G28,IF(TYPE(climbs!G28)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=8.6</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H28)=2,CHAR(34),""),climbs!H28,IF(TYPE(climbs!H28)=2,CHAR(34),""))</f>
+        <v>CATEGORY="3"</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A29)=2,CHAR(34),""),climbs!A29,IF(TYPE(climbs!A29)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=28</v>
@@ -3736,8 +3844,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G29)=2,CHAR(34),""),climbs!G29,IF(TYPE(climbs!G29)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=5.4</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H29)=2,CHAR(34),""),climbs!H29,IF(TYPE(climbs!H29)=2,CHAR(34),""))</f>
+        <v>CATEGORY="2"</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A30)=2,CHAR(34),""),climbs!A30,IF(TYPE(climbs!A30)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=29</v>
@@ -3766,8 +3878,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G30)=2,CHAR(34),""),climbs!G30,IF(TYPE(climbs!G30)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=8.1</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H30)=2,CHAR(34),""),climbs!H30,IF(TYPE(climbs!H30)=2,CHAR(34),""))</f>
+        <v>CATEGORY="1"</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A31)=2,CHAR(34),""),climbs!A31,IF(TYPE(climbs!A31)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=30</v>
@@ -3796,8 +3912,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G31)=2,CHAR(34),""),climbs!G31,IF(TYPE(climbs!G31)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=8.4</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H31)=2,CHAR(34),""),climbs!H31,IF(TYPE(climbs!H31)=2,CHAR(34),""))</f>
+        <v>CATEGORY="1"</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A32)=2,CHAR(34),""),climbs!A32,IF(TYPE(climbs!A32)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=31</v>
@@ -3826,8 +3946,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G32)=2,CHAR(34),""),climbs!G32,IF(TYPE(climbs!G32)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=6.1</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H32)=2,CHAR(34),""),climbs!H32,IF(TYPE(climbs!H32)=2,CHAR(34),""))</f>
+        <v>CATEGORY="2"</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A33)=2,CHAR(34),""),climbs!A33,IF(TYPE(climbs!A33)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=32</v>
@@ -3856,8 +3980,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G33)=2,CHAR(34),""),climbs!G33,IF(TYPE(climbs!G33)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=6.2</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H33" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H33)=2,CHAR(34),""),climbs!H33,IF(TYPE(climbs!H33)=2,CHAR(34),""))</f>
+        <v>CATEGORY="3"</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A34)=2,CHAR(34),""),climbs!A34,IF(TYPE(climbs!A34)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=33</v>
@@ -3886,8 +4014,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G34)=2,CHAR(34),""),climbs!G34,IF(TYPE(climbs!G34)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=9.5</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H34)=2,CHAR(34),""),climbs!H34,IF(TYPE(climbs!H34)=2,CHAR(34),""))</f>
+        <v>CATEGORY="1"</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A35)=2,CHAR(34),""),climbs!A35,IF(TYPE(climbs!A35)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=34</v>
@@ -3916,8 +4048,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G35)=2,CHAR(34),""),climbs!G35,IF(TYPE(climbs!G35)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=8.5</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H35" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H35)=2,CHAR(34),""),climbs!H35,IF(TYPE(climbs!H35)=2,CHAR(34),""))</f>
+        <v>CATEGORY="1"</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A36)=2,CHAR(34),""),climbs!A36,IF(TYPE(climbs!A36)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=35</v>
@@ -3946,8 +4082,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G36)=2,CHAR(34),""),climbs!G36,IF(TYPE(climbs!G36)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=4.9</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H36" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H36)=2,CHAR(34),""),climbs!H36,IF(TYPE(climbs!H36)=2,CHAR(34),""))</f>
+        <v>CATEGORY="3"</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A37)=2,CHAR(34),""),climbs!A37,IF(TYPE(climbs!A37)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=36</v>
@@ -3976,8 +4116,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G37)=2,CHAR(34),""),climbs!G37,IF(TYPE(climbs!G37)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=6.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H37" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H37)=2,CHAR(34),""),climbs!H37,IF(TYPE(climbs!H37)=2,CHAR(34),""))</f>
+        <v>CATEGORY="3"</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A38)=2,CHAR(34),""),climbs!A38,IF(TYPE(climbs!A38)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=37</v>
@@ -4006,8 +4150,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G38)=2,CHAR(34),""),climbs!G38,IF(TYPE(climbs!G38)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=5.2</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H38" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H38)=2,CHAR(34),""),climbs!H38,IF(TYPE(climbs!H38)=2,CHAR(34),""))</f>
+        <v>CATEGORY="4"</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A39)=2,CHAR(34),""),climbs!A39,IF(TYPE(climbs!A39)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=38</v>
@@ -4036,8 +4184,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G39)=2,CHAR(34),""),climbs!G39,IF(TYPE(climbs!G39)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=6.6</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H39" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H39)=2,CHAR(34),""),climbs!H39,IF(TYPE(climbs!H39)=2,CHAR(34),""))</f>
+        <v>CATEGORY="3"</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A40)=2,CHAR(34),""),climbs!A40,IF(TYPE(climbs!A40)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=39</v>
@@ -4066,8 +4218,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G40)=2,CHAR(34),""),climbs!G40,IF(TYPE(climbs!G40)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=5.1</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H40" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H40)=2,CHAR(34),""),climbs!H40,IF(TYPE(climbs!H40)=2,CHAR(34),""))</f>
+        <v>CATEGORY="4"</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A41)=2,CHAR(34),""),climbs!A41,IF(TYPE(climbs!A41)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=40</v>
@@ -4096,8 +4252,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G41)=2,CHAR(34),""),climbs!G41,IF(TYPE(climbs!G41)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=4.5</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H41" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H41)=2,CHAR(34),""),climbs!H41,IF(TYPE(climbs!H41)=2,CHAR(34),""))</f>
+        <v>CATEGORY="3"</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A42)=2,CHAR(34),""),climbs!A42,IF(TYPE(climbs!A42)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=41</v>
@@ -4126,8 +4286,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G42)=2,CHAR(34),""),climbs!G42,IF(TYPE(climbs!G42)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=3.3</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H42" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H42)=2,CHAR(34),""),climbs!H42,IF(TYPE(climbs!H42)=2,CHAR(34),""))</f>
+        <v>CATEGORY="3"</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A43)=2,CHAR(34),""),climbs!A43,IF(TYPE(climbs!A43)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=42</v>
@@ -4156,8 +4320,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G43)=2,CHAR(34),""),climbs!G43,IF(TYPE(climbs!G43)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=2.9</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H43" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H43)=2,CHAR(34),""),climbs!H43,IF(TYPE(climbs!H43)=2,CHAR(34),""))</f>
+        <v>CATEGORY="4"</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A44)=2,CHAR(34),""),climbs!A44,IF(TYPE(climbs!A44)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=43</v>
@@ -4186,8 +4354,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G44)=2,CHAR(34),""),climbs!G44,IF(TYPE(climbs!G44)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=4.1</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H44" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H44)=2,CHAR(34),""),climbs!H44,IF(TYPE(climbs!H44)=2,CHAR(34),""))</f>
+        <v>CATEGORY="3"</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A45)=2,CHAR(34),""),climbs!A45,IF(TYPE(climbs!A45)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=44</v>
@@ -4216,8 +4388,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G45)=2,CHAR(34),""),climbs!G45,IF(TYPE(climbs!G45)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=6.1</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H45" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H45)=2,CHAR(34),""),climbs!H45,IF(TYPE(climbs!H45)=2,CHAR(34),""))</f>
+        <v>CATEGORY="1"</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A46)=2,CHAR(34),""),climbs!A46,IF(TYPE(climbs!A46)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=45</v>
@@ -4246,8 +4422,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G46)=2,CHAR(34),""),climbs!G46,IF(TYPE(climbs!G46)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=7.3</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H46" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H46)=2,CHAR(34),""),climbs!H46,IF(TYPE(climbs!H46)=2,CHAR(34),""))</f>
+        <v>CATEGORY="H"</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A47)=2,CHAR(34),""),climbs!A47,IF(TYPE(climbs!A47)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=46</v>
@@ -4276,8 +4456,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G47)=2,CHAR(34),""),climbs!G47,IF(TYPE(climbs!G47)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=3.9</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H47" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H47)=2,CHAR(34),""),climbs!H47,IF(TYPE(climbs!H47)=2,CHAR(34),""))</f>
+        <v>CATEGORY="1"</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A48)=2,CHAR(34),""),climbs!A48,IF(TYPE(climbs!A48)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=47</v>
@@ -4306,8 +4490,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G48)=2,CHAR(34),""),climbs!G48,IF(TYPE(climbs!G48)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=6</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H48" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H48)=2,CHAR(34),""),climbs!H48,IF(TYPE(climbs!H48)=2,CHAR(34),""))</f>
+        <v>CATEGORY="H"</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A49)=2,CHAR(34),""),climbs!A49,IF(TYPE(climbs!A49)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=48</v>
@@ -4336,8 +4524,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G49)=2,CHAR(34),""),climbs!G49,IF(TYPE(climbs!G49)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=6.9</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H49" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H49)=2,CHAR(34),""),climbs!H49,IF(TYPE(climbs!H49)=2,CHAR(34),""))</f>
+        <v>CATEGORY="1"</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A50)=2,CHAR(34),""),climbs!A50,IF(TYPE(climbs!A50)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=49</v>
@@ -4366,8 +4558,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G50)=2,CHAR(34),""),climbs!G50,IF(TYPE(climbs!G50)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=4.9</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H50" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H50)=2,CHAR(34),""),climbs!H50,IF(TYPE(climbs!H50)=2,CHAR(34),""))</f>
+        <v>CATEGORY="4"</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A51)=2,CHAR(34),""),climbs!A51,IF(TYPE(climbs!A51)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=50</v>
@@ -4396,8 +4592,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G51)=2,CHAR(34),""),climbs!G51,IF(TYPE(climbs!G51)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=5.4</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H51" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H51)=2,CHAR(34),""),climbs!H51,IF(TYPE(climbs!H51)=2,CHAR(34),""))</f>
+        <v>CATEGORY="4"</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A52)=2,CHAR(34),""),climbs!A52,IF(TYPE(climbs!A52)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=51</v>
@@ -4426,8 +4626,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G52)=2,CHAR(34),""),climbs!G52,IF(TYPE(climbs!G52)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=6.9</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H52" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H52)=2,CHAR(34),""),climbs!H52,IF(TYPE(climbs!H52)=2,CHAR(34),""))</f>
+        <v>CATEGORY="2"</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A53)=2,CHAR(34),""),climbs!A53,IF(TYPE(climbs!A53)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=52</v>
@@ -4456,8 +4660,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G53)=2,CHAR(34),""),climbs!G53,IF(TYPE(climbs!G53)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=5.2</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H53" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H53)=2,CHAR(34),""),climbs!H53,IF(TYPE(climbs!H53)=2,CHAR(34),""))</f>
+        <v>CATEGORY="3"</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A54)=2,CHAR(34),""),climbs!A54,IF(TYPE(climbs!A54)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=53</v>
@@ -4486,8 +4694,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G54)=2,CHAR(34),""),climbs!G54,IF(TYPE(climbs!G54)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=7.7</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H54" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H54)=2,CHAR(34),""),climbs!H54,IF(TYPE(climbs!H54)=2,CHAR(34),""))</f>
+        <v>CATEGORY="H"</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A55)=2,CHAR(34),""),climbs!A55,IF(TYPE(climbs!A55)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=54</v>
@@ -4516,8 +4728,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G55)=2,CHAR(34),""),climbs!G55,IF(TYPE(climbs!G55)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=7.1</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H55" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H55)=2,CHAR(34),""),climbs!H55,IF(TYPE(climbs!H55)=2,CHAR(34),""))</f>
+        <v>CATEGORY="1"</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A56)=2,CHAR(34),""),climbs!A56,IF(TYPE(climbs!A56)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=55</v>
@@ -4546,8 +4762,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G56)=2,CHAR(34),""),climbs!G56,IF(TYPE(climbs!G56)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=7</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H56" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H56)=2,CHAR(34),""),climbs!H56,IF(TYPE(climbs!H56)=2,CHAR(34),""))</f>
+        <v>CATEGORY="1"</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A57)=2,CHAR(34),""),climbs!A57,IF(TYPE(climbs!A57)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=56</v>
@@ -4576,8 +4796,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G57)=2,CHAR(34),""),climbs!G57,IF(TYPE(climbs!G57)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=8.3</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H57" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H57)=2,CHAR(34),""),climbs!H57,IF(TYPE(climbs!H57)=2,CHAR(34),""))</f>
+        <v>CATEGORY="1"</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A58)=2,CHAR(34),""),climbs!A58,IF(TYPE(climbs!A58)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=57</v>
@@ -4606,8 +4830,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G58)=2,CHAR(34),""),climbs!G58,IF(TYPE(climbs!G58)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=8.3</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H58" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H58)=2,CHAR(34),""),climbs!H58,IF(TYPE(climbs!H58)=2,CHAR(34),""))</f>
+        <v>CATEGORY="H"</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A59)=2,CHAR(34),""),climbs!A59,IF(TYPE(climbs!A59)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=58</v>
@@ -4636,8 +4864,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G59)=2,CHAR(34),""),climbs!G59,IF(TYPE(climbs!G59)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=6.7</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H59" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H59)=2,CHAR(34),""),climbs!H59,IF(TYPE(climbs!H59)=2,CHAR(34),""))</f>
+        <v>CATEGORY="3"</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A60)=2,CHAR(34),""),climbs!A60,IF(TYPE(climbs!A60)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=59</v>
@@ -4666,8 +4898,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G60)=2,CHAR(34),""),climbs!G60,IF(TYPE(climbs!G60)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=7</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H60" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H60)=2,CHAR(34),""),climbs!H60,IF(TYPE(climbs!H60)=2,CHAR(34),""))</f>
+        <v>CATEGORY="3"</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A61)=2,CHAR(34),""),climbs!A61,IF(TYPE(climbs!A61)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=60</v>
@@ -4696,8 +4932,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G61)=2,CHAR(34),""),climbs!G61,IF(TYPE(climbs!G61)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=7.3</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H61" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H61)=2,CHAR(34),""),climbs!H61,IF(TYPE(climbs!H61)=2,CHAR(34),""))</f>
+        <v>CATEGORY="H"</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A62)=2,CHAR(34),""),climbs!A62,IF(TYPE(climbs!A62)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=61</v>
@@ -4726,8 +4966,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G62)=2,CHAR(34),""),climbs!G62,IF(TYPE(climbs!G62)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=7.8</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H62" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H62)=2,CHAR(34),""),climbs!H62,IF(TYPE(climbs!H62)=2,CHAR(34),""))</f>
+        <v>CATEGORY="H"</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A63)=2,CHAR(34),""),climbs!A63,IF(TYPE(climbs!A63)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=62</v>
@@ -4756,8 +5000,12 @@
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G63)=2,CHAR(34),""),climbs!G63,IF(TYPE(climbs!G63)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=7.6</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H63" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H63)=2,CHAR(34),""),climbs!H63,IF(TYPE(climbs!H63)=2,CHAR(34),""))</f>
+        <v>CATEGORY="4"</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
         <f>CONCATENATE(climbs!A$1, "=",IF(TYPE(climbs!A64)=2,CHAR(34),""),climbs!A64,IF(TYPE(climbs!A64)=2,CHAR(34),""))</f>
         <v>CLIMB_ID=63</v>
@@ -4785,6 +5033,10 @@
       <c r="G64" t="str">
         <f>CONCATENATE(climbs!G$1, "=",IF(TYPE(climbs!G64)=2,CHAR(34),""),climbs!G64,IF(TYPE(climbs!G64)=2,CHAR(34),""))</f>
         <v>AVERAGE_SLOPE=0</v>
+      </c>
+      <c r="H64" t="str">
+        <f>CONCATENATE(climbs!H$1, "=",IF(TYPE(climbs!H64)=2,CHAR(34),""),climbs!H64,IF(TYPE(climbs!H64)=2,CHAR(34),""))</f>
+        <v>CATEGORY="4"</v>
       </c>
     </row>
   </sheetData>
@@ -4796,7 +5048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A64"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A64"/>
     </sheetView>
   </sheetViews>
@@ -4812,380 +5064,380 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A2:G2)</f>
-        <v>CLIMB_ID=1, STAGE_NUMBER=1, STARTING_AT_KM=68, NAME="Côte de Cray", INITIAL_ALTITUDE=0, DISTANCE=1.6, AVERAGE_SLOPE=7.1</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A2:H2)</f>
+        <v>CLIMB_ID=1, STAGE_NUMBER=1, STARTING_AT_KM=68, NAME="Côte de Cray", INITIAL_ALTITUDE=0, DISTANCE=1.6, AVERAGE_SLOPE=7.1, CATEGORY="4"</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A3:G3)</f>
-        <v>CLIMB_ID=2, STAGE_NUMBER=1, STARTING_AT_KM=103.5, NAME="Côte de Buttertubs", INITIAL_ALTITUDE=0, DISTANCE=4.5, AVERAGE_SLOPE=6.8</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A3:H3)</f>
+        <v>CLIMB_ID=2, STAGE_NUMBER=1, STARTING_AT_KM=103.5, NAME="Côte de Buttertubs", INITIAL_ALTITUDE=0, DISTANCE=4.5, AVERAGE_SLOPE=6.8, CATEGORY="3"</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A4:G4)</f>
-        <v>CLIMB_ID=3, STAGE_NUMBER=1, STARTING_AT_KM=129.5, NAME="Côte de Griton Moor", INITIAL_ALTITUDE=0, DISTANCE=3, AVERAGE_SLOPE=6.6</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A4:H4)</f>
+        <v>CLIMB_ID=3, STAGE_NUMBER=1, STARTING_AT_KM=129.5, NAME="Côte de Griton Moor", INITIAL_ALTITUDE=0, DISTANCE=3, AVERAGE_SLOPE=6.6, CATEGORY="3"</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A5:G5)</f>
-        <v>CLIMB_ID=4, STAGE_NUMBER=2, STARTING_AT_KM=47, NAME="Côte de Blubberhouses", INITIAL_ALTITUDE=0, DISTANCE=1.8, AVERAGE_SLOPE=6.1</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A5:H5)</f>
+        <v>CLIMB_ID=4, STAGE_NUMBER=2, STARTING_AT_KM=47, NAME="Côte de Blubberhouses", INITIAL_ALTITUDE=0, DISTANCE=1.8, AVERAGE_SLOPE=6.1, CATEGORY="4"</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A6:G6)</f>
-        <v>CLIMB_ID=5, STAGE_NUMBER=2, STARTING_AT_KM=85, NAME="Côte d'Oxenhope Moor", INITIAL_ALTITUDE=0, DISTANCE=3.1, AVERAGE_SLOPE=6.4</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A6:H6)</f>
+        <v>CLIMB_ID=5, STAGE_NUMBER=2, STARTING_AT_KM=85, NAME="Côte d'Oxenhope Moor", INITIAL_ALTITUDE=0, DISTANCE=3.1, AVERAGE_SLOPE=6.4, CATEGORY="3"</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A7:G7)</f>
-        <v>CLIMB_ID=6, STAGE_NUMBER=2, STARTING_AT_KM=112.5, NAME="VC Côte de Ripponden", INITIAL_ALTITUDE=0, DISTANCE=1.3, AVERAGE_SLOPE=8.6</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A7:H7)</f>
+        <v>CLIMB_ID=6, STAGE_NUMBER=2, STARTING_AT_KM=112.5, NAME="VC Côte de Ripponden", INITIAL_ALTITUDE=0, DISTANCE=1.3, AVERAGE_SLOPE=8.6, CATEGORY="3"</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A8:G8)</f>
-        <v>CLIMB_ID=7, STAGE_NUMBER=2, STARTING_AT_KM=119.5, NAME="Côte de Greetland", INITIAL_ALTITUDE=0, DISTANCE=1.6, AVERAGE_SLOPE=6.7</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A8:H8)</f>
+        <v>CLIMB_ID=7, STAGE_NUMBER=2, STARTING_AT_KM=119.5, NAME="Côte de Greetland", INITIAL_ALTITUDE=0, DISTANCE=1.6, AVERAGE_SLOPE=6.7, CATEGORY="3"</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A9:G9)</f>
-        <v>CLIMB_ID=8, STAGE_NUMBER=2, STARTING_AT_KM=143.5, NAME="Côte de Holme Moss", INITIAL_ALTITUDE=0, DISTANCE=4.7, AVERAGE_SLOPE=7</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A9:H9)</f>
+        <v>CLIMB_ID=8, STAGE_NUMBER=2, STARTING_AT_KM=143.5, NAME="Côte de Holme Moss", INITIAL_ALTITUDE=0, DISTANCE=4.7, AVERAGE_SLOPE=7, CATEGORY="2"</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A10:G10)</f>
-        <v>CLIMB_ID=9, STAGE_NUMBER=2, STARTING_AT_KM=167, NAME="Côte de Midhopestones", INITIAL_ALTITUDE=0, DISTANCE=2.5, AVERAGE_SLOPE=6.1</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A10:H10)</f>
+        <v>CLIMB_ID=9, STAGE_NUMBER=2, STARTING_AT_KM=167, NAME="Côte de Midhopestones", INITIAL_ALTITUDE=0, DISTANCE=2.5, AVERAGE_SLOPE=6.1, CATEGORY="3"</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A11:G11)</f>
-        <v>CLIMB_ID=10, STAGE_NUMBER=2, STARTING_AT_KM=175, NAME="Côte de Bradfield", INITIAL_ALTITUDE=0, DISTANCE=1, AVERAGE_SLOPE=7.4</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A11:H11)</f>
+        <v>CLIMB_ID=10, STAGE_NUMBER=2, STARTING_AT_KM=175, NAME="Côte de Bradfield", INITIAL_ALTITUDE=0, DISTANCE=1, AVERAGE_SLOPE=7.4, CATEGORY="4"</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A12:G12)</f>
-        <v>CLIMB_ID=11, STAGE_NUMBER=2, STARTING_AT_KM=182, NAME="Côte d'Oughtibridge", INITIAL_ALTITUDE=0, DISTANCE=1.5, AVERAGE_SLOPE=9.1</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A12:H12)</f>
+        <v>CLIMB_ID=11, STAGE_NUMBER=2, STARTING_AT_KM=182, NAME="Côte d'Oughtibridge", INITIAL_ALTITUDE=0, DISTANCE=1.5, AVERAGE_SLOPE=9.1, CATEGORY="3"</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A13:G13)</f>
-        <v>CLIMB_ID=12, STAGE_NUMBER=2, STARTING_AT_KM=196, NAME="VC Côte de Jenkin Road", INITIAL_ALTITUDE=0, DISTANCE=0.8, AVERAGE_SLOPE=10.8</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A13:H13)</f>
+        <v>CLIMB_ID=12, STAGE_NUMBER=2, STARTING_AT_KM=196, NAME="VC Côte de Jenkin Road", INITIAL_ALTITUDE=0, DISTANCE=0.8, AVERAGE_SLOPE=10.8, CATEGORY="4"</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A14:G14)</f>
-        <v>CLIMB_ID=13, STAGE_NUMBER=4, STARTING_AT_KM=34, NAME="Côte de Campagnette", INITIAL_ALTITUDE=0, DISTANCE=1, AVERAGE_SLOPE=6.5</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A14:H14)</f>
+        <v>CLIMB_ID=13, STAGE_NUMBER=4, STARTING_AT_KM=34, NAME="Côte de Campagnette", INITIAL_ALTITUDE=0, DISTANCE=1, AVERAGE_SLOPE=6.5, CATEGORY="4"</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A15:G15)</f>
-        <v>CLIMB_ID=14, STAGE_NUMBER=4, STARTING_AT_KM=117.5, NAME="Mont Noir", INITIAL_ALTITUDE=0, DISTANCE=1.3, AVERAGE_SLOPE=5.7</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A15:H15)</f>
+        <v>CLIMB_ID=14, STAGE_NUMBER=4, STARTING_AT_KM=117.5, NAME="Mont Noir", INITIAL_ALTITUDE=0, DISTANCE=1.3, AVERAGE_SLOPE=5.7, CATEGORY="4"</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A16:G16)</f>
-        <v>CLIMB_ID=15, STAGE_NUMBER=6, STARTING_AT_KM=107.5, NAME="Côte de Coucy-le-Château-Auffrique", INITIAL_ALTITUDE=0, DISTANCE=0.9, AVERAGE_SLOPE=6.2</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A16:H16)</f>
+        <v>CLIMB_ID=15, STAGE_NUMBER=6, STARTING_AT_KM=107.5, NAME="Côte de Coucy-le-Château-Auffrique", INITIAL_ALTITUDE=0, DISTANCE=0.9, AVERAGE_SLOPE=6.2, CATEGORY="4"</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A17:G17)</f>
-        <v>CLIMB_ID=16, STAGE_NUMBER=6, STARTING_AT_KM=157, NAME="Côte de Roucy", INITIAL_ALTITUDE=0, DISTANCE=1.5, AVERAGE_SLOPE=6.2</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A17:H17)</f>
+        <v>CLIMB_ID=16, STAGE_NUMBER=6, STARTING_AT_KM=157, NAME="Côte de Roucy", INITIAL_ALTITUDE=0, DISTANCE=1.5, AVERAGE_SLOPE=6.2, CATEGORY="4"</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A18:G18)</f>
-        <v>CLIMB_ID=17, STAGE_NUMBER=7, STARTING_AT_KM=217.5, NAME="Côte de Maron", INITIAL_ALTITUDE=0, DISTANCE=3.2, AVERAGE_SLOPE=5</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A18:H18)</f>
+        <v>CLIMB_ID=17, STAGE_NUMBER=7, STARTING_AT_KM=217.5, NAME="Côte de Maron", INITIAL_ALTITUDE=0, DISTANCE=3.2, AVERAGE_SLOPE=5, CATEGORY="4"</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A19:G19)</f>
-        <v>CLIMB_ID=18, STAGE_NUMBER=7, STARTING_AT_KM=229, NAME="Côte de Boufflers", INITIAL_ALTITUDE=0, DISTANCE=1.3, AVERAGE_SLOPE=7.9</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A19:H19)</f>
+        <v>CLIMB_ID=18, STAGE_NUMBER=7, STARTING_AT_KM=229, NAME="Côte de Boufflers", INITIAL_ALTITUDE=0, DISTANCE=1.3, AVERAGE_SLOPE=7.9, CATEGORY="4"</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A20:G20)</f>
-        <v>CLIMB_ID=19, STAGE_NUMBER=8, STARTING_AT_KM=142, NAME="Col de la Croix des Moinats", INITIAL_ALTITUDE=891, DISTANCE=7.6, AVERAGE_SLOPE=6</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A20:H20)</f>
+        <v>CLIMB_ID=19, STAGE_NUMBER=8, STARTING_AT_KM=142, NAME="Col de la Croix des Moinats", INITIAL_ALTITUDE=891, DISTANCE=7.6, AVERAGE_SLOPE=6, CATEGORY="2"</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A21:G21)</f>
-        <v>CLIMB_ID=20, STAGE_NUMBER=8, STARTING_AT_KM=150, NAME="Col de Grosse Pierre", INITIAL_ALTITUDE=901, DISTANCE=3, AVERAGE_SLOPE=7.5</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A21:H21)</f>
+        <v>CLIMB_ID=20, STAGE_NUMBER=8, STARTING_AT_KM=150, NAME="Col de Grosse Pierre", INITIAL_ALTITUDE=901, DISTANCE=3, AVERAGE_SLOPE=7.5, CATEGORY="2"</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A22:G22)</f>
-        <v>CLIMB_ID=21, STAGE_NUMBER=8, STARTING_AT_KM=161, NAME="Côte de La Mauselaine", INITIAL_ALTITUDE=0, DISTANCE=1.8, AVERAGE_SLOPE=10.3</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A22:H22)</f>
+        <v>CLIMB_ID=21, STAGE_NUMBER=8, STARTING_AT_KM=161, NAME="Côte de La Mauselaine", INITIAL_ALTITUDE=0, DISTANCE=1.8, AVERAGE_SLOPE=10.3, CATEGORY="3"</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A23:G23)</f>
-        <v>CLIMB_ID=22, STAGE_NUMBER=9, STARTING_AT_KM=11.5, NAME="Col de la Schlucht", INITIAL_ALTITUDE=1140, DISTANCE=8.6, AVERAGE_SLOPE=4.5</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A23:H23)</f>
+        <v>CLIMB_ID=22, STAGE_NUMBER=9, STARTING_AT_KM=11.5, NAME="Col de la Schlucht", INITIAL_ALTITUDE=1140, DISTANCE=8.6, AVERAGE_SLOPE=4.5, CATEGORY="2"</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A24:G24)</f>
-        <v>CLIMB_ID=23, STAGE_NUMBER=9, STARTING_AT_KM=41, NAME="Col du Wettstein", INITIAL_ALTITUDE=0, DISTANCE=7.7, AVERAGE_SLOPE=4.1</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A24:H24)</f>
+        <v>CLIMB_ID=23, STAGE_NUMBER=9, STARTING_AT_KM=41, NAME="Col du Wettstein", INITIAL_ALTITUDE=0, DISTANCE=7.7, AVERAGE_SLOPE=4.1, CATEGORY="3"</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A25:G25)</f>
-        <v>CLIMB_ID=24, STAGE_NUMBER=9, STARTING_AT_KM=70, NAME="Côte des Cinq Châteaux", INITIAL_ALTITUDE=0, DISTANCE=4.5, AVERAGE_SLOPE=6.1</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A25:H25)</f>
+        <v>CLIMB_ID=24, STAGE_NUMBER=9, STARTING_AT_KM=70, NAME="Côte des Cinq Châteaux", INITIAL_ALTITUDE=0, DISTANCE=4.5, AVERAGE_SLOPE=6.1, CATEGORY="3"</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A26:G26)</f>
-        <v>CLIMB_ID=25, STAGE_NUMBER=9, STARTING_AT_KM=86, NAME="Côte de Gueberschwihr", INITIAL_ALTITUDE=559, DISTANCE=4.1, AVERAGE_SLOPE=7.9</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A26:H26)</f>
+        <v>CLIMB_ID=25, STAGE_NUMBER=9, STARTING_AT_KM=86, NAME="Côte de Gueberschwihr", INITIAL_ALTITUDE=559, DISTANCE=4.1, AVERAGE_SLOPE=7.9, CATEGORY="2"</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A27:G27)</f>
-        <v>CLIMB_ID=26, STAGE_NUMBER=9, STARTING_AT_KM=120, NAME="Le Markstein", INITIAL_ALTITUDE=1183, DISTANCE=10.8, AVERAGE_SLOPE=5.4</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A27:H27)</f>
+        <v>CLIMB_ID=26, STAGE_NUMBER=9, STARTING_AT_KM=120, NAME="Le Markstein", INITIAL_ALTITUDE=1183, DISTANCE=10.8, AVERAGE_SLOPE=5.4, CATEGORY="1"</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A28:G28)</f>
-        <v>CLIMB_ID=27, STAGE_NUMBER=9, STARTING_AT_KM=127, NAME="Grand Ballon", INITIAL_ALTITUDE=0, DISTANCE=1.4, AVERAGE_SLOPE=8.6</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A28:H28)</f>
+        <v>CLIMB_ID=27, STAGE_NUMBER=9, STARTING_AT_KM=127, NAME="Grand Ballon", INITIAL_ALTITUDE=0, DISTANCE=1.4, AVERAGE_SLOPE=8.6, CATEGORY="3"</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A29:G29)</f>
-        <v>CLIMB_ID=28, STAGE_NUMBER=10, STARTING_AT_KM=30.5, NAME="Col du Firstplan", INITIAL_ALTITUDE=722, DISTANCE=8.3, AVERAGE_SLOPE=5.4</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A29:H29)</f>
+        <v>CLIMB_ID=28, STAGE_NUMBER=10, STARTING_AT_KM=30.5, NAME="Col du Firstplan", INITIAL_ALTITUDE=722, DISTANCE=8.3, AVERAGE_SLOPE=5.4, CATEGORY="2"</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A30:G30)</f>
-        <v>CLIMB_ID=29, STAGE_NUMBER=10, STARTING_AT_KM=54.5, NAME="Petit Ballon", INITIAL_ALTITUDE=1163, DISTANCE=9.3, AVERAGE_SLOPE=8.1</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A30:H30)</f>
+        <v>CLIMB_ID=29, STAGE_NUMBER=10, STARTING_AT_KM=54.5, NAME="Petit Ballon", INITIAL_ALTITUDE=1163, DISTANCE=9.3, AVERAGE_SLOPE=8.1, CATEGORY="1"</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A31:G31)</f>
-        <v>CLIMB_ID=30, STAGE_NUMBER=10, STARTING_AT_KM=71.5, NAME="Col du Platzerwasel", INITIAL_ALTITUDE=1193, DISTANCE=7.1, AVERAGE_SLOPE=8.4</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A31:H31)</f>
+        <v>CLIMB_ID=30, STAGE_NUMBER=10, STARTING_AT_KM=71.5, NAME="Col du Platzerwasel", INITIAL_ALTITUDE=1193, DISTANCE=7.1, AVERAGE_SLOPE=8.4, CATEGORY="1"</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A32:G32)</f>
-        <v>CLIMB_ID=31, STAGE_NUMBER=10, STARTING_AT_KM=103.5, NAME="Col d'Oderen", INITIAL_ALTITUDE=884, DISTANCE=6.7, AVERAGE_SLOPE=6.1</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A32:H32)</f>
+        <v>CLIMB_ID=31, STAGE_NUMBER=10, STARTING_AT_KM=103.5, NAME="Col d'Oderen", INITIAL_ALTITUDE=884, DISTANCE=6.7, AVERAGE_SLOPE=6.1, CATEGORY="2"</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A33:G33)</f>
-        <v>CLIMB_ID=32, STAGE_NUMBER=10, STARTING_AT_KM=125.5, NAME="Col des Croix", INITIAL_ALTITUDE=0, DISTANCE=3.2, AVERAGE_SLOPE=6.2</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A33:H33)</f>
+        <v>CLIMB_ID=32, STAGE_NUMBER=10, STARTING_AT_KM=125.5, NAME="Col des Croix", INITIAL_ALTITUDE=0, DISTANCE=3.2, AVERAGE_SLOPE=6.2, CATEGORY="3"</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A34:G34)</f>
-        <v>CLIMB_ID=33, STAGE_NUMBER=10, STARTING_AT_KM=143.5, NAME="Col des Chevrères", INITIAL_ALTITUDE=914, DISTANCE=3.5, AVERAGE_SLOPE=9.5</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A34:H34)</f>
+        <v>CLIMB_ID=33, STAGE_NUMBER=10, STARTING_AT_KM=143.5, NAME="Col des Chevrères", INITIAL_ALTITUDE=914, DISTANCE=3.5, AVERAGE_SLOPE=9.5, CATEGORY="1"</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A35:G35)</f>
-        <v>CLIMB_ID=34, STAGE_NUMBER=10, STARTING_AT_KM=161.5, NAME="La Planche des Belles Filles", INITIAL_ALTITUDE=1035, DISTANCE=5.9, AVERAGE_SLOPE=8.5</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A35:H35)</f>
+        <v>CLIMB_ID=34, STAGE_NUMBER=10, STARTING_AT_KM=161.5, NAME="La Planche des Belles Filles", INITIAL_ALTITUDE=1035, DISTANCE=5.9, AVERAGE_SLOPE=8.5, CATEGORY="1"</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A36:G36)</f>
-        <v>CLIMB_ID=35, STAGE_NUMBER=11, STARTING_AT_KM=141, NAME="Côte de Rogna", INITIAL_ALTITUDE=0, DISTANCE=7.6, AVERAGE_SLOPE=4.9</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A36:H36)</f>
+        <v>CLIMB_ID=35, STAGE_NUMBER=11, STARTING_AT_KM=141, NAME="Côte de Rogna", INITIAL_ALTITUDE=0, DISTANCE=7.6, AVERAGE_SLOPE=4.9, CATEGORY="3"</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A37:G37)</f>
-        <v>CLIMB_ID=36, STAGE_NUMBER=11, STARTING_AT_KM=148.5, NAME="Côte de Choux", INITIAL_ALTITUDE=0, DISTANCE=1.7, AVERAGE_SLOPE=6.5</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A37:H37)</f>
+        <v>CLIMB_ID=36, STAGE_NUMBER=11, STARTING_AT_KM=148.5, NAME="Côte de Choux", INITIAL_ALTITUDE=0, DISTANCE=1.7, AVERAGE_SLOPE=6.5, CATEGORY="3"</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A38:G38)</f>
-        <v>CLIMB_ID=37, STAGE_NUMBER=11, STARTING_AT_KM=152.5, NAME="Côte de Désertin", INITIAL_ALTITUDE=0, DISTANCE=3.1, AVERAGE_SLOPE=5.2</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A38:H38)</f>
+        <v>CLIMB_ID=37, STAGE_NUMBER=11, STARTING_AT_KM=152.5, NAME="Côte de Désertin", INITIAL_ALTITUDE=0, DISTANCE=3.1, AVERAGE_SLOPE=5.2, CATEGORY="4"</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A39:G39)</f>
-        <v>CLIMB_ID=38, STAGE_NUMBER=11, STARTING_AT_KM=168, NAME="Côte d'Échallon", INITIAL_ALTITUDE=0, DISTANCE=3, AVERAGE_SLOPE=6.6</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A39:H39)</f>
+        <v>CLIMB_ID=38, STAGE_NUMBER=11, STARTING_AT_KM=168, NAME="Côte d'Échallon", INITIAL_ALTITUDE=0, DISTANCE=3, AVERAGE_SLOPE=6.6, CATEGORY="3"</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A40:G40)</f>
-        <v>CLIMB_ID=39, STAGE_NUMBER=12, STARTING_AT_KM=58.5, NAME="Col de Brouilly", INITIAL_ALTITUDE=0, DISTANCE=1.7, AVERAGE_SLOPE=5.1</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A40:H40)</f>
+        <v>CLIMB_ID=39, STAGE_NUMBER=12, STARTING_AT_KM=58.5, NAME="Col de Brouilly", INITIAL_ALTITUDE=0, DISTANCE=1.7, AVERAGE_SLOPE=5.1, CATEGORY="4"</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A41:G41)</f>
-        <v>CLIMB_ID=40, STAGE_NUMBER=12, STARTING_AT_KM=83, NAME="Côte du Saule-d'Oingt", INITIAL_ALTITUDE=0, DISTANCE=3.8, AVERAGE_SLOPE=4.5</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A41:H41)</f>
+        <v>CLIMB_ID=40, STAGE_NUMBER=12, STARTING_AT_KM=83, NAME="Côte du Saule-d'Oingt", INITIAL_ALTITUDE=0, DISTANCE=3.8, AVERAGE_SLOPE=4.5, CATEGORY="3"</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A42:G42)</f>
-        <v>CLIMB_ID=41, STAGE_NUMBER=12, STARTING_AT_KM=138, NAME="Col des Brosses", INITIAL_ALTITUDE=0, DISTANCE=15.3, AVERAGE_SLOPE=3.3</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A42:H42)</f>
+        <v>CLIMB_ID=41, STAGE_NUMBER=12, STARTING_AT_KM=138, NAME="Col des Brosses", INITIAL_ALTITUDE=0, DISTANCE=15.3, AVERAGE_SLOPE=3.3, CATEGORY="3"</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A43:G43)</f>
-        <v>CLIMB_ID=42, STAGE_NUMBER=12, STARTING_AT_KM=164, NAME="Côte de Grammond", INITIAL_ALTITUDE=0, DISTANCE=9.8, AVERAGE_SLOPE=2.9</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A43:H43)</f>
+        <v>CLIMB_ID=42, STAGE_NUMBER=12, STARTING_AT_KM=164, NAME="Côte de Grammond", INITIAL_ALTITUDE=0, DISTANCE=9.8, AVERAGE_SLOPE=2.9, CATEGORY="4"</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A44:G44)</f>
-        <v>CLIMB_ID=43, STAGE_NUMBER=13, STARTING_AT_KM=24, NAME="Col de la Croix de Montvieux", INITIAL_ALTITUDE=0, DISTANCE=8, AVERAGE_SLOPE=4.1</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A44:H44)</f>
+        <v>CLIMB_ID=43, STAGE_NUMBER=13, STARTING_AT_KM=24, NAME="Col de la Croix de Montvieux", INITIAL_ALTITUDE=0, DISTANCE=8, AVERAGE_SLOPE=4.1, CATEGORY="3"</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A45:G45)</f>
-        <v>CLIMB_ID=44, STAGE_NUMBER=13, STARTING_AT_KM=152, NAME="Col de Palaquit (D57-D512)", INITIAL_ALTITUDE=1154, DISTANCE=14.1, AVERAGE_SLOPE=6.1</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A45:H45)</f>
+        <v>CLIMB_ID=44, STAGE_NUMBER=13, STARTING_AT_KM=152, NAME="Col de Palaquit (D57-D512)", INITIAL_ALTITUDE=1154, DISTANCE=14.1, AVERAGE_SLOPE=6.1, CATEGORY="1"</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A46:G46)</f>
-        <v>CLIMB_ID=45, STAGE_NUMBER=13, STARTING_AT_KM=197.5, NAME="Montée de Chamrousse", INITIAL_ALTITUDE=1730, DISTANCE=18.2, AVERAGE_SLOPE=7.3</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A46:H46)</f>
+        <v>CLIMB_ID=45, STAGE_NUMBER=13, STARTING_AT_KM=197.5, NAME="Montée de Chamrousse", INITIAL_ALTITUDE=1730, DISTANCE=18.2, AVERAGE_SLOPE=7.3, CATEGORY="H"</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A47:G47)</f>
-        <v>CLIMB_ID=46, STAGE_NUMBER=14, STARTING_AT_KM=82, NAME="Col du Lautaret", INITIAL_ALTITUDE=2058, DISTANCE=34, AVERAGE_SLOPE=3.9</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A47:H47)</f>
+        <v>CLIMB_ID=46, STAGE_NUMBER=14, STARTING_AT_KM=82, NAME="Col du Lautaret", INITIAL_ALTITUDE=2058, DISTANCE=34, AVERAGE_SLOPE=3.9, CATEGORY="1"</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A48:G48)</f>
-        <v>CLIMB_ID=47, STAGE_NUMBER=14, STARTING_AT_KM=132.5, NAME="Col d'Izoard - Souvenir Henri Desgrange", INITIAL_ALTITUDE=2360, DISTANCE=19, AVERAGE_SLOPE=6</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A48:H48)</f>
+        <v>CLIMB_ID=47, STAGE_NUMBER=14, STARTING_AT_KM=132.5, NAME="Col d'Izoard - Souvenir Henri Desgrange", INITIAL_ALTITUDE=2360, DISTANCE=19, AVERAGE_SLOPE=6, CATEGORY="H"</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A49:G49)</f>
-        <v>CLIMB_ID=48, STAGE_NUMBER=14, STARTING_AT_KM=177, NAME="Montée de Risoul", INITIAL_ALTITUDE=1855, DISTANCE=12.6, AVERAGE_SLOPE=6.9</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A49:H49)</f>
+        <v>CLIMB_ID=48, STAGE_NUMBER=14, STARTING_AT_KM=177, NAME="Montée de Risoul", INITIAL_ALTITUDE=1855, DISTANCE=12.6, AVERAGE_SLOPE=6.9, CATEGORY="1"</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A50:G50)</f>
-        <v>CLIMB_ID=49, STAGE_NUMBER=16, STARTING_AT_KM=25, NAME="Côte de Fanjeaux", INITIAL_ALTITUDE=0, DISTANCE=2.4, AVERAGE_SLOPE=4.9</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A50:H50)</f>
+        <v>CLIMB_ID=49, STAGE_NUMBER=16, STARTING_AT_KM=25, NAME="Côte de Fanjeaux", INITIAL_ALTITUDE=0, DISTANCE=2.4, AVERAGE_SLOPE=4.9, CATEGORY="4"</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A51:G51)</f>
-        <v>CLIMB_ID=50, STAGE_NUMBER=16, STARTING_AT_KM=71.5, NAME="Côte de Pamiers", INITIAL_ALTITUDE=0, DISTANCE=2.5, AVERAGE_SLOPE=5.4</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A51:H51)</f>
+        <v>CLIMB_ID=50, STAGE_NUMBER=16, STARTING_AT_KM=71.5, NAME="Côte de Pamiers", INITIAL_ALTITUDE=0, DISTANCE=2.5, AVERAGE_SLOPE=5.4, CATEGORY="4"</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A52:G52)</f>
-        <v>CLIMB_ID=51, STAGE_NUMBER=16, STARTING_AT_KM=155, NAME="Col de Portet-d'Aspet", INITIAL_ALTITUDE=1069, DISTANCE=5.4, AVERAGE_SLOPE=6.9</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A52:H52)</f>
+        <v>CLIMB_ID=51, STAGE_NUMBER=16, STARTING_AT_KM=155, NAME="Col de Portet-d'Aspet", INITIAL_ALTITUDE=1069, DISTANCE=5.4, AVERAGE_SLOPE=6.9, CATEGORY="2"</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A53:G53)</f>
-        <v>CLIMB_ID=52, STAGE_NUMBER=16, STARTING_AT_KM=176.5, NAME="Col des Ares", INITIAL_ALTITUDE=0, DISTANCE=6, AVERAGE_SLOPE=5.2</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A53:H53)</f>
+        <v>CLIMB_ID=52, STAGE_NUMBER=16, STARTING_AT_KM=176.5, NAME="Col des Ares", INITIAL_ALTITUDE=0, DISTANCE=6, AVERAGE_SLOPE=5.2, CATEGORY="3"</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A54:G54)</f>
-        <v>CLIMB_ID=53, STAGE_NUMBER=16, STARTING_AT_KM=216, NAME="Port de Balès", INITIAL_ALTITUDE=1755, DISTANCE=11.7, AVERAGE_SLOPE=7.7</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A54:H54)</f>
+        <v>CLIMB_ID=53, STAGE_NUMBER=16, STARTING_AT_KM=216, NAME="Port de Balès", INITIAL_ALTITUDE=1755, DISTANCE=11.7, AVERAGE_SLOPE=7.7, CATEGORY="H"</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A55:G55)</f>
-        <v>CLIMB_ID=54, STAGE_NUMBER=17, STARTING_AT_KM=57.5, NAME="Col du Portillon", INITIAL_ALTITUDE=1292, DISTANCE=8.3, AVERAGE_SLOPE=7.1</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A55:H55)</f>
+        <v>CLIMB_ID=54, STAGE_NUMBER=17, STARTING_AT_KM=57.5, NAME="Col du Portillon", INITIAL_ALTITUDE=1292, DISTANCE=8.3, AVERAGE_SLOPE=7.1, CATEGORY="1"</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A56:G56)</f>
-        <v>CLIMB_ID=55, STAGE_NUMBER=17, STARTING_AT_KM=82, NAME="Col de Peyresourde", INITIAL_ALTITUDE=1569, DISTANCE=13.2, AVERAGE_SLOPE=7</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A56:H56)</f>
+        <v>CLIMB_ID=55, STAGE_NUMBER=17, STARTING_AT_KM=82, NAME="Col de Peyresourde", INITIAL_ALTITUDE=1569, DISTANCE=13.2, AVERAGE_SLOPE=7, CATEGORY="1"</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A57:G57)</f>
-        <v>CLIMB_ID=56, STAGE_NUMBER=17, STARTING_AT_KM=102.5, NAME="Col de Val Louron-Azet", INITIAL_ALTITUDE=1580, DISTANCE=7.4, AVERAGE_SLOPE=8.3</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A57:H57)</f>
+        <v>CLIMB_ID=56, STAGE_NUMBER=17, STARTING_AT_KM=102.5, NAME="Col de Val Louron-Azet", INITIAL_ALTITUDE=1580, DISTANCE=7.4, AVERAGE_SLOPE=8.3, CATEGORY="1"</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A58:G58)</f>
-        <v>CLIMB_ID=57, STAGE_NUMBER=17, STARTING_AT_KM=124.5, NAME="Montée de Saint-Lary Pla d'Adet", INITIAL_ALTITUDE=1680, DISTANCE=10.2, AVERAGE_SLOPE=8.3</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A58:H58)</f>
+        <v>CLIMB_ID=57, STAGE_NUMBER=17, STARTING_AT_KM=124.5, NAME="Montée de Saint-Lary Pla d'Adet", INITIAL_ALTITUDE=1680, DISTANCE=10.2, AVERAGE_SLOPE=8.3, CATEGORY="H"</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A59:G59)</f>
-        <v>CLIMB_ID=58, STAGE_NUMBER=18, STARTING_AT_KM=28, NAME="Côte de Bénéjacq", INITIAL_ALTITUDE=0, DISTANCE=2.6, AVERAGE_SLOPE=6.7</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A59:H59)</f>
+        <v>CLIMB_ID=58, STAGE_NUMBER=18, STARTING_AT_KM=28, NAME="Côte de Bénéjacq", INITIAL_ALTITUDE=0, DISTANCE=2.6, AVERAGE_SLOPE=6.7, CATEGORY="3"</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A60:G60)</f>
-        <v>CLIMB_ID=59, STAGE_NUMBER=18, STARTING_AT_KM=56, NAME="Côte de Loucrup", INITIAL_ALTITUDE=0, DISTANCE=2, AVERAGE_SLOPE=7</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A60:H60)</f>
+        <v>CLIMB_ID=59, STAGE_NUMBER=18, STARTING_AT_KM=56, NAME="Côte de Loucrup", INITIAL_ALTITUDE=0, DISTANCE=2, AVERAGE_SLOPE=7, CATEGORY="3"</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A61:G61)</f>
-        <v>CLIMB_ID=60, STAGE_NUMBER=18, STARTING_AT_KM=95.5, NAME="Col du Tourmalet - Souvenir Jacques Goddet", INITIAL_ALTITUDE=2115, DISTANCE=17.1, AVERAGE_SLOPE=7.3</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A61:H61)</f>
+        <v>CLIMB_ID=60, STAGE_NUMBER=18, STARTING_AT_KM=95.5, NAME="Col du Tourmalet - Souvenir Jacques Goddet", INITIAL_ALTITUDE=2115, DISTANCE=17.1, AVERAGE_SLOPE=7.3, CATEGORY="H"</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A62:G62)</f>
-        <v>CLIMB_ID=61, STAGE_NUMBER=18, STARTING_AT_KM=145.5, NAME="Montée du Hautacam", INITIAL_ALTITUDE=1520, DISTANCE=13.6, AVERAGE_SLOPE=7.8</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A62:H62)</f>
+        <v>CLIMB_ID=61, STAGE_NUMBER=18, STARTING_AT_KM=145.5, NAME="Montée du Hautacam", INITIAL_ALTITUDE=1520, DISTANCE=13.6, AVERAGE_SLOPE=7.8, CATEGORY="H"</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A63:G63)</f>
-        <v>CLIMB_ID=62, STAGE_NUMBER=19, STARTING_AT_KM=195.5, NAME="Côte de Monbazillac", INITIAL_ALTITUDE=0, DISTANCE=1.3, AVERAGE_SLOPE=7.6</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A63:H63)</f>
+        <v>CLIMB_ID=62, STAGE_NUMBER=19, STARTING_AT_KM=195.5, NAME="Côte de Monbazillac", INITIAL_ALTITUDE=0, DISTANCE=1.3, AVERAGE_SLOPE=7.6, CATEGORY="4"</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
-        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A64:G64)</f>
-        <v>CLIMB_ID=63, STAGE_NUMBER=21, STARTING_AT_KM=31, NAME="Côte de Briis-sous-Forges", INITIAL_ALTITUDE=0, DISTANCE=0, AVERAGE_SLOPE=0</v>
+        <f>_xlfn.TEXTJOIN(", ", TRUE, 'fields &amp; values'!A64:H64)</f>
+        <v>CLIMB_ID=63, STAGE_NUMBER=21, STARTING_AT_KM=31, NAME="Côte de Briis-sous-Forges", INITIAL_ALTITUDE=0, DISTANCE=0, AVERAGE_SLOPE=0, CATEGORY="4"</v>
       </c>
     </row>
   </sheetData>
@@ -5197,7 +5449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A64"/>
     </sheetView>
   </sheetViews>
@@ -5211,379 +5463,379 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A2, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=1, STAGE_NUMBER=1, STARTING_AT_KM=68, NAME="Côte de Cray", INITIAL_ALTITUDE=0, DISTANCE=1.6, AVERAGE_SLOPE=7.1;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=1, STAGE_NUMBER=1, STARTING_AT_KM=68, NAME="Côte de Cray", INITIAL_ALTITUDE=0, DISTANCE=1.6, AVERAGE_SLOPE=7.1, CATEGORY="4";</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A3, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=2, STAGE_NUMBER=1, STARTING_AT_KM=103.5, NAME="Côte de Buttertubs", INITIAL_ALTITUDE=0, DISTANCE=4.5, AVERAGE_SLOPE=6.8;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=2, STAGE_NUMBER=1, STARTING_AT_KM=103.5, NAME="Côte de Buttertubs", INITIAL_ALTITUDE=0, DISTANCE=4.5, AVERAGE_SLOPE=6.8, CATEGORY="3";</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A4, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=3, STAGE_NUMBER=1, STARTING_AT_KM=129.5, NAME="Côte de Griton Moor", INITIAL_ALTITUDE=0, DISTANCE=3, AVERAGE_SLOPE=6.6;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=3, STAGE_NUMBER=1, STARTING_AT_KM=129.5, NAME="Côte de Griton Moor", INITIAL_ALTITUDE=0, DISTANCE=3, AVERAGE_SLOPE=6.6, CATEGORY="3";</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A5, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=4, STAGE_NUMBER=2, STARTING_AT_KM=47, NAME="Côte de Blubberhouses", INITIAL_ALTITUDE=0, DISTANCE=1.8, AVERAGE_SLOPE=6.1;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=4, STAGE_NUMBER=2, STARTING_AT_KM=47, NAME="Côte de Blubberhouses", INITIAL_ALTITUDE=0, DISTANCE=1.8, AVERAGE_SLOPE=6.1, CATEGORY="4";</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A6, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=5, STAGE_NUMBER=2, STARTING_AT_KM=85, NAME="Côte d'Oxenhope Moor", INITIAL_ALTITUDE=0, DISTANCE=3.1, AVERAGE_SLOPE=6.4;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=5, STAGE_NUMBER=2, STARTING_AT_KM=85, NAME="Côte d'Oxenhope Moor", INITIAL_ALTITUDE=0, DISTANCE=3.1, AVERAGE_SLOPE=6.4, CATEGORY="3";</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A7, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=6, STAGE_NUMBER=2, STARTING_AT_KM=112.5, NAME="VC Côte de Ripponden", INITIAL_ALTITUDE=0, DISTANCE=1.3, AVERAGE_SLOPE=8.6;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=6, STAGE_NUMBER=2, STARTING_AT_KM=112.5, NAME="VC Côte de Ripponden", INITIAL_ALTITUDE=0, DISTANCE=1.3, AVERAGE_SLOPE=8.6, CATEGORY="3";</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A8, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=7, STAGE_NUMBER=2, STARTING_AT_KM=119.5, NAME="Côte de Greetland", INITIAL_ALTITUDE=0, DISTANCE=1.6, AVERAGE_SLOPE=6.7;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=7, STAGE_NUMBER=2, STARTING_AT_KM=119.5, NAME="Côte de Greetland", INITIAL_ALTITUDE=0, DISTANCE=1.6, AVERAGE_SLOPE=6.7, CATEGORY="3";</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A9, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=8, STAGE_NUMBER=2, STARTING_AT_KM=143.5, NAME="Côte de Holme Moss", INITIAL_ALTITUDE=0, DISTANCE=4.7, AVERAGE_SLOPE=7;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=8, STAGE_NUMBER=2, STARTING_AT_KM=143.5, NAME="Côte de Holme Moss", INITIAL_ALTITUDE=0, DISTANCE=4.7, AVERAGE_SLOPE=7, CATEGORY="2";</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A10, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=9, STAGE_NUMBER=2, STARTING_AT_KM=167, NAME="Côte de Midhopestones", INITIAL_ALTITUDE=0, DISTANCE=2.5, AVERAGE_SLOPE=6.1;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=9, STAGE_NUMBER=2, STARTING_AT_KM=167, NAME="Côte de Midhopestones", INITIAL_ALTITUDE=0, DISTANCE=2.5, AVERAGE_SLOPE=6.1, CATEGORY="3";</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A11, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=10, STAGE_NUMBER=2, STARTING_AT_KM=175, NAME="Côte de Bradfield", INITIAL_ALTITUDE=0, DISTANCE=1, AVERAGE_SLOPE=7.4;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=10, STAGE_NUMBER=2, STARTING_AT_KM=175, NAME="Côte de Bradfield", INITIAL_ALTITUDE=0, DISTANCE=1, AVERAGE_SLOPE=7.4, CATEGORY="4";</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A12, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=11, STAGE_NUMBER=2, STARTING_AT_KM=182, NAME="Côte d'Oughtibridge", INITIAL_ALTITUDE=0, DISTANCE=1.5, AVERAGE_SLOPE=9.1;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=11, STAGE_NUMBER=2, STARTING_AT_KM=182, NAME="Côte d'Oughtibridge", INITIAL_ALTITUDE=0, DISTANCE=1.5, AVERAGE_SLOPE=9.1, CATEGORY="3";</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A13, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=12, STAGE_NUMBER=2, STARTING_AT_KM=196, NAME="VC Côte de Jenkin Road", INITIAL_ALTITUDE=0, DISTANCE=0.8, AVERAGE_SLOPE=10.8;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=12, STAGE_NUMBER=2, STARTING_AT_KM=196, NAME="VC Côte de Jenkin Road", INITIAL_ALTITUDE=0, DISTANCE=0.8, AVERAGE_SLOPE=10.8, CATEGORY="4";</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A14, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=13, STAGE_NUMBER=4, STARTING_AT_KM=34, NAME="Côte de Campagnette", INITIAL_ALTITUDE=0, DISTANCE=1, AVERAGE_SLOPE=6.5;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=13, STAGE_NUMBER=4, STARTING_AT_KM=34, NAME="Côte de Campagnette", INITIAL_ALTITUDE=0, DISTANCE=1, AVERAGE_SLOPE=6.5, CATEGORY="4";</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A15, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=14, STAGE_NUMBER=4, STARTING_AT_KM=117.5, NAME="Mont Noir", INITIAL_ALTITUDE=0, DISTANCE=1.3, AVERAGE_SLOPE=5.7;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=14, STAGE_NUMBER=4, STARTING_AT_KM=117.5, NAME="Mont Noir", INITIAL_ALTITUDE=0, DISTANCE=1.3, AVERAGE_SLOPE=5.7, CATEGORY="4";</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A16, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=15, STAGE_NUMBER=6, STARTING_AT_KM=107.5, NAME="Côte de Coucy-le-Château-Auffrique", INITIAL_ALTITUDE=0, DISTANCE=0.9, AVERAGE_SLOPE=6.2;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=15, STAGE_NUMBER=6, STARTING_AT_KM=107.5, NAME="Côte de Coucy-le-Château-Auffrique", INITIAL_ALTITUDE=0, DISTANCE=0.9, AVERAGE_SLOPE=6.2, CATEGORY="4";</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A17, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=16, STAGE_NUMBER=6, STARTING_AT_KM=157, NAME="Côte de Roucy", INITIAL_ALTITUDE=0, DISTANCE=1.5, AVERAGE_SLOPE=6.2;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=16, STAGE_NUMBER=6, STARTING_AT_KM=157, NAME="Côte de Roucy", INITIAL_ALTITUDE=0, DISTANCE=1.5, AVERAGE_SLOPE=6.2, CATEGORY="4";</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A18, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=17, STAGE_NUMBER=7, STARTING_AT_KM=217.5, NAME="Côte de Maron", INITIAL_ALTITUDE=0, DISTANCE=3.2, AVERAGE_SLOPE=5;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=17, STAGE_NUMBER=7, STARTING_AT_KM=217.5, NAME="Côte de Maron", INITIAL_ALTITUDE=0, DISTANCE=3.2, AVERAGE_SLOPE=5, CATEGORY="4";</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A19, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=18, STAGE_NUMBER=7, STARTING_AT_KM=229, NAME="Côte de Boufflers", INITIAL_ALTITUDE=0, DISTANCE=1.3, AVERAGE_SLOPE=7.9;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=18, STAGE_NUMBER=7, STARTING_AT_KM=229, NAME="Côte de Boufflers", INITIAL_ALTITUDE=0, DISTANCE=1.3, AVERAGE_SLOPE=7.9, CATEGORY="4";</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A20, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=19, STAGE_NUMBER=8, STARTING_AT_KM=142, NAME="Col de la Croix des Moinats", INITIAL_ALTITUDE=891, DISTANCE=7.6, AVERAGE_SLOPE=6;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=19, STAGE_NUMBER=8, STARTING_AT_KM=142, NAME="Col de la Croix des Moinats", INITIAL_ALTITUDE=891, DISTANCE=7.6, AVERAGE_SLOPE=6, CATEGORY="2";</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A21, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=20, STAGE_NUMBER=8, STARTING_AT_KM=150, NAME="Col de Grosse Pierre", INITIAL_ALTITUDE=901, DISTANCE=3, AVERAGE_SLOPE=7.5;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=20, STAGE_NUMBER=8, STARTING_AT_KM=150, NAME="Col de Grosse Pierre", INITIAL_ALTITUDE=901, DISTANCE=3, AVERAGE_SLOPE=7.5, CATEGORY="2";</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A22, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=21, STAGE_NUMBER=8, STARTING_AT_KM=161, NAME="Côte de La Mauselaine", INITIAL_ALTITUDE=0, DISTANCE=1.8, AVERAGE_SLOPE=10.3;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=21, STAGE_NUMBER=8, STARTING_AT_KM=161, NAME="Côte de La Mauselaine", INITIAL_ALTITUDE=0, DISTANCE=1.8, AVERAGE_SLOPE=10.3, CATEGORY="3";</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A23, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=22, STAGE_NUMBER=9, STARTING_AT_KM=11.5, NAME="Col de la Schlucht", INITIAL_ALTITUDE=1140, DISTANCE=8.6, AVERAGE_SLOPE=4.5;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=22, STAGE_NUMBER=9, STARTING_AT_KM=11.5, NAME="Col de la Schlucht", INITIAL_ALTITUDE=1140, DISTANCE=8.6, AVERAGE_SLOPE=4.5, CATEGORY="2";</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A24, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=23, STAGE_NUMBER=9, STARTING_AT_KM=41, NAME="Col du Wettstein", INITIAL_ALTITUDE=0, DISTANCE=7.7, AVERAGE_SLOPE=4.1;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=23, STAGE_NUMBER=9, STARTING_AT_KM=41, NAME="Col du Wettstein", INITIAL_ALTITUDE=0, DISTANCE=7.7, AVERAGE_SLOPE=4.1, CATEGORY="3";</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A25, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=24, STAGE_NUMBER=9, STARTING_AT_KM=70, NAME="Côte des Cinq Châteaux", INITIAL_ALTITUDE=0, DISTANCE=4.5, AVERAGE_SLOPE=6.1;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=24, STAGE_NUMBER=9, STARTING_AT_KM=70, NAME="Côte des Cinq Châteaux", INITIAL_ALTITUDE=0, DISTANCE=4.5, AVERAGE_SLOPE=6.1, CATEGORY="3";</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A26, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=25, STAGE_NUMBER=9, STARTING_AT_KM=86, NAME="Côte de Gueberschwihr", INITIAL_ALTITUDE=559, DISTANCE=4.1, AVERAGE_SLOPE=7.9;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=25, STAGE_NUMBER=9, STARTING_AT_KM=86, NAME="Côte de Gueberschwihr", INITIAL_ALTITUDE=559, DISTANCE=4.1, AVERAGE_SLOPE=7.9, CATEGORY="2";</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A27, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=26, STAGE_NUMBER=9, STARTING_AT_KM=120, NAME="Le Markstein", INITIAL_ALTITUDE=1183, DISTANCE=10.8, AVERAGE_SLOPE=5.4;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=26, STAGE_NUMBER=9, STARTING_AT_KM=120, NAME="Le Markstein", INITIAL_ALTITUDE=1183, DISTANCE=10.8, AVERAGE_SLOPE=5.4, CATEGORY="1";</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A28, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=27, STAGE_NUMBER=9, STARTING_AT_KM=127, NAME="Grand Ballon", INITIAL_ALTITUDE=0, DISTANCE=1.4, AVERAGE_SLOPE=8.6;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=27, STAGE_NUMBER=9, STARTING_AT_KM=127, NAME="Grand Ballon", INITIAL_ALTITUDE=0, DISTANCE=1.4, AVERAGE_SLOPE=8.6, CATEGORY="3";</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A29, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=28, STAGE_NUMBER=10, STARTING_AT_KM=30.5, NAME="Col du Firstplan", INITIAL_ALTITUDE=722, DISTANCE=8.3, AVERAGE_SLOPE=5.4;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=28, STAGE_NUMBER=10, STARTING_AT_KM=30.5, NAME="Col du Firstplan", INITIAL_ALTITUDE=722, DISTANCE=8.3, AVERAGE_SLOPE=5.4, CATEGORY="2";</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A30, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=29, STAGE_NUMBER=10, STARTING_AT_KM=54.5, NAME="Petit Ballon", INITIAL_ALTITUDE=1163, DISTANCE=9.3, AVERAGE_SLOPE=8.1;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=29, STAGE_NUMBER=10, STARTING_AT_KM=54.5, NAME="Petit Ballon", INITIAL_ALTITUDE=1163, DISTANCE=9.3, AVERAGE_SLOPE=8.1, CATEGORY="1";</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A31, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=30, STAGE_NUMBER=10, STARTING_AT_KM=71.5, NAME="Col du Platzerwasel", INITIAL_ALTITUDE=1193, DISTANCE=7.1, AVERAGE_SLOPE=8.4;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=30, STAGE_NUMBER=10, STARTING_AT_KM=71.5, NAME="Col du Platzerwasel", INITIAL_ALTITUDE=1193, DISTANCE=7.1, AVERAGE_SLOPE=8.4, CATEGORY="1";</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A32, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=31, STAGE_NUMBER=10, STARTING_AT_KM=103.5, NAME="Col d'Oderen", INITIAL_ALTITUDE=884, DISTANCE=6.7, AVERAGE_SLOPE=6.1;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=31, STAGE_NUMBER=10, STARTING_AT_KM=103.5, NAME="Col d'Oderen", INITIAL_ALTITUDE=884, DISTANCE=6.7, AVERAGE_SLOPE=6.1, CATEGORY="2";</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A33, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=32, STAGE_NUMBER=10, STARTING_AT_KM=125.5, NAME="Col des Croix", INITIAL_ALTITUDE=0, DISTANCE=3.2, AVERAGE_SLOPE=6.2;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=32, STAGE_NUMBER=10, STARTING_AT_KM=125.5, NAME="Col des Croix", INITIAL_ALTITUDE=0, DISTANCE=3.2, AVERAGE_SLOPE=6.2, CATEGORY="3";</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A34, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=33, STAGE_NUMBER=10, STARTING_AT_KM=143.5, NAME="Col des Chevrères", INITIAL_ALTITUDE=914, DISTANCE=3.5, AVERAGE_SLOPE=9.5;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=33, STAGE_NUMBER=10, STARTING_AT_KM=143.5, NAME="Col des Chevrères", INITIAL_ALTITUDE=914, DISTANCE=3.5, AVERAGE_SLOPE=9.5, CATEGORY="1";</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A35, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=34, STAGE_NUMBER=10, STARTING_AT_KM=161.5, NAME="La Planche des Belles Filles", INITIAL_ALTITUDE=1035, DISTANCE=5.9, AVERAGE_SLOPE=8.5;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=34, STAGE_NUMBER=10, STARTING_AT_KM=161.5, NAME="La Planche des Belles Filles", INITIAL_ALTITUDE=1035, DISTANCE=5.9, AVERAGE_SLOPE=8.5, CATEGORY="1";</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A36, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=35, STAGE_NUMBER=11, STARTING_AT_KM=141, NAME="Côte de Rogna", INITIAL_ALTITUDE=0, DISTANCE=7.6, AVERAGE_SLOPE=4.9;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=35, STAGE_NUMBER=11, STARTING_AT_KM=141, NAME="Côte de Rogna", INITIAL_ALTITUDE=0, DISTANCE=7.6, AVERAGE_SLOPE=4.9, CATEGORY="3";</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A37, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=36, STAGE_NUMBER=11, STARTING_AT_KM=148.5, NAME="Côte de Choux", INITIAL_ALTITUDE=0, DISTANCE=1.7, AVERAGE_SLOPE=6.5;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=36, STAGE_NUMBER=11, STARTING_AT_KM=148.5, NAME="Côte de Choux", INITIAL_ALTITUDE=0, DISTANCE=1.7, AVERAGE_SLOPE=6.5, CATEGORY="3";</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A38, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=37, STAGE_NUMBER=11, STARTING_AT_KM=152.5, NAME="Côte de Désertin", INITIAL_ALTITUDE=0, DISTANCE=3.1, AVERAGE_SLOPE=5.2;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=37, STAGE_NUMBER=11, STARTING_AT_KM=152.5, NAME="Côte de Désertin", INITIAL_ALTITUDE=0, DISTANCE=3.1, AVERAGE_SLOPE=5.2, CATEGORY="4";</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A39, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=38, STAGE_NUMBER=11, STARTING_AT_KM=168, NAME="Côte d'Échallon", INITIAL_ALTITUDE=0, DISTANCE=3, AVERAGE_SLOPE=6.6;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=38, STAGE_NUMBER=11, STARTING_AT_KM=168, NAME="Côte d'Échallon", INITIAL_ALTITUDE=0, DISTANCE=3, AVERAGE_SLOPE=6.6, CATEGORY="3";</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A40, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=39, STAGE_NUMBER=12, STARTING_AT_KM=58.5, NAME="Col de Brouilly", INITIAL_ALTITUDE=0, DISTANCE=1.7, AVERAGE_SLOPE=5.1;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=39, STAGE_NUMBER=12, STARTING_AT_KM=58.5, NAME="Col de Brouilly", INITIAL_ALTITUDE=0, DISTANCE=1.7, AVERAGE_SLOPE=5.1, CATEGORY="4";</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A41, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=40, STAGE_NUMBER=12, STARTING_AT_KM=83, NAME="Côte du Saule-d'Oingt", INITIAL_ALTITUDE=0, DISTANCE=3.8, AVERAGE_SLOPE=4.5;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=40, STAGE_NUMBER=12, STARTING_AT_KM=83, NAME="Côte du Saule-d'Oingt", INITIAL_ALTITUDE=0, DISTANCE=3.8, AVERAGE_SLOPE=4.5, CATEGORY="3";</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A42, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=41, STAGE_NUMBER=12, STARTING_AT_KM=138, NAME="Col des Brosses", INITIAL_ALTITUDE=0, DISTANCE=15.3, AVERAGE_SLOPE=3.3;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=41, STAGE_NUMBER=12, STARTING_AT_KM=138, NAME="Col des Brosses", INITIAL_ALTITUDE=0, DISTANCE=15.3, AVERAGE_SLOPE=3.3, CATEGORY="3";</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A43, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=42, STAGE_NUMBER=12, STARTING_AT_KM=164, NAME="Côte de Grammond", INITIAL_ALTITUDE=0, DISTANCE=9.8, AVERAGE_SLOPE=2.9;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=42, STAGE_NUMBER=12, STARTING_AT_KM=164, NAME="Côte de Grammond", INITIAL_ALTITUDE=0, DISTANCE=9.8, AVERAGE_SLOPE=2.9, CATEGORY="4";</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A44, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=43, STAGE_NUMBER=13, STARTING_AT_KM=24, NAME="Col de la Croix de Montvieux", INITIAL_ALTITUDE=0, DISTANCE=8, AVERAGE_SLOPE=4.1;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=43, STAGE_NUMBER=13, STARTING_AT_KM=24, NAME="Col de la Croix de Montvieux", INITIAL_ALTITUDE=0, DISTANCE=8, AVERAGE_SLOPE=4.1, CATEGORY="3";</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A45, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=44, STAGE_NUMBER=13, STARTING_AT_KM=152, NAME="Col de Palaquit (D57-D512)", INITIAL_ALTITUDE=1154, DISTANCE=14.1, AVERAGE_SLOPE=6.1;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=44, STAGE_NUMBER=13, STARTING_AT_KM=152, NAME="Col de Palaquit (D57-D512)", INITIAL_ALTITUDE=1154, DISTANCE=14.1, AVERAGE_SLOPE=6.1, CATEGORY="1";</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A46, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=45, STAGE_NUMBER=13, STARTING_AT_KM=197.5, NAME="Montée de Chamrousse", INITIAL_ALTITUDE=1730, DISTANCE=18.2, AVERAGE_SLOPE=7.3;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=45, STAGE_NUMBER=13, STARTING_AT_KM=197.5, NAME="Montée de Chamrousse", INITIAL_ALTITUDE=1730, DISTANCE=18.2, AVERAGE_SLOPE=7.3, CATEGORY="H";</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A47, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=46, STAGE_NUMBER=14, STARTING_AT_KM=82, NAME="Col du Lautaret", INITIAL_ALTITUDE=2058, DISTANCE=34, AVERAGE_SLOPE=3.9;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=46, STAGE_NUMBER=14, STARTING_AT_KM=82, NAME="Col du Lautaret", INITIAL_ALTITUDE=2058, DISTANCE=34, AVERAGE_SLOPE=3.9, CATEGORY="1";</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A48, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=47, STAGE_NUMBER=14, STARTING_AT_KM=132.5, NAME="Col d'Izoard - Souvenir Henri Desgrange", INITIAL_ALTITUDE=2360, DISTANCE=19, AVERAGE_SLOPE=6;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=47, STAGE_NUMBER=14, STARTING_AT_KM=132.5, NAME="Col d'Izoard - Souvenir Henri Desgrange", INITIAL_ALTITUDE=2360, DISTANCE=19, AVERAGE_SLOPE=6, CATEGORY="H";</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A49, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=48, STAGE_NUMBER=14, STARTING_AT_KM=177, NAME="Montée de Risoul", INITIAL_ALTITUDE=1855, DISTANCE=12.6, AVERAGE_SLOPE=6.9;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=48, STAGE_NUMBER=14, STARTING_AT_KM=177, NAME="Montée de Risoul", INITIAL_ALTITUDE=1855, DISTANCE=12.6, AVERAGE_SLOPE=6.9, CATEGORY="1";</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A50, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=49, STAGE_NUMBER=16, STARTING_AT_KM=25, NAME="Côte de Fanjeaux", INITIAL_ALTITUDE=0, DISTANCE=2.4, AVERAGE_SLOPE=4.9;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=49, STAGE_NUMBER=16, STARTING_AT_KM=25, NAME="Côte de Fanjeaux", INITIAL_ALTITUDE=0, DISTANCE=2.4, AVERAGE_SLOPE=4.9, CATEGORY="4";</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A51, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=50, STAGE_NUMBER=16, STARTING_AT_KM=71.5, NAME="Côte de Pamiers", INITIAL_ALTITUDE=0, DISTANCE=2.5, AVERAGE_SLOPE=5.4;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=50, STAGE_NUMBER=16, STARTING_AT_KM=71.5, NAME="Côte de Pamiers", INITIAL_ALTITUDE=0, DISTANCE=2.5, AVERAGE_SLOPE=5.4, CATEGORY="4";</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A52, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=51, STAGE_NUMBER=16, STARTING_AT_KM=155, NAME="Col de Portet-d'Aspet", INITIAL_ALTITUDE=1069, DISTANCE=5.4, AVERAGE_SLOPE=6.9;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=51, STAGE_NUMBER=16, STARTING_AT_KM=155, NAME="Col de Portet-d'Aspet", INITIAL_ALTITUDE=1069, DISTANCE=5.4, AVERAGE_SLOPE=6.9, CATEGORY="2";</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A53, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=52, STAGE_NUMBER=16, STARTING_AT_KM=176.5, NAME="Col des Ares", INITIAL_ALTITUDE=0, DISTANCE=6, AVERAGE_SLOPE=5.2;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=52, STAGE_NUMBER=16, STARTING_AT_KM=176.5, NAME="Col des Ares", INITIAL_ALTITUDE=0, DISTANCE=6, AVERAGE_SLOPE=5.2, CATEGORY="3";</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A54, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=53, STAGE_NUMBER=16, STARTING_AT_KM=216, NAME="Port de Balès", INITIAL_ALTITUDE=1755, DISTANCE=11.7, AVERAGE_SLOPE=7.7;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=53, STAGE_NUMBER=16, STARTING_AT_KM=216, NAME="Port de Balès", INITIAL_ALTITUDE=1755, DISTANCE=11.7, AVERAGE_SLOPE=7.7, CATEGORY="H";</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A55, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=54, STAGE_NUMBER=17, STARTING_AT_KM=57.5, NAME="Col du Portillon", INITIAL_ALTITUDE=1292, DISTANCE=8.3, AVERAGE_SLOPE=7.1;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=54, STAGE_NUMBER=17, STARTING_AT_KM=57.5, NAME="Col du Portillon", INITIAL_ALTITUDE=1292, DISTANCE=8.3, AVERAGE_SLOPE=7.1, CATEGORY="1";</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A56, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=55, STAGE_NUMBER=17, STARTING_AT_KM=82, NAME="Col de Peyresourde", INITIAL_ALTITUDE=1569, DISTANCE=13.2, AVERAGE_SLOPE=7;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=55, STAGE_NUMBER=17, STARTING_AT_KM=82, NAME="Col de Peyresourde", INITIAL_ALTITUDE=1569, DISTANCE=13.2, AVERAGE_SLOPE=7, CATEGORY="1";</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A57, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=56, STAGE_NUMBER=17, STARTING_AT_KM=102.5, NAME="Col de Val Louron-Azet", INITIAL_ALTITUDE=1580, DISTANCE=7.4, AVERAGE_SLOPE=8.3;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=56, STAGE_NUMBER=17, STARTING_AT_KM=102.5, NAME="Col de Val Louron-Azet", INITIAL_ALTITUDE=1580, DISTANCE=7.4, AVERAGE_SLOPE=8.3, CATEGORY="1";</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A58, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=57, STAGE_NUMBER=17, STARTING_AT_KM=124.5, NAME="Montée de Saint-Lary Pla d'Adet", INITIAL_ALTITUDE=1680, DISTANCE=10.2, AVERAGE_SLOPE=8.3;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=57, STAGE_NUMBER=17, STARTING_AT_KM=124.5, NAME="Montée de Saint-Lary Pla d'Adet", INITIAL_ALTITUDE=1680, DISTANCE=10.2, AVERAGE_SLOPE=8.3, CATEGORY="H";</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A59, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=58, STAGE_NUMBER=18, STARTING_AT_KM=28, NAME="Côte de Bénéjacq", INITIAL_ALTITUDE=0, DISTANCE=2.6, AVERAGE_SLOPE=6.7;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=58, STAGE_NUMBER=18, STARTING_AT_KM=28, NAME="Côte de Bénéjacq", INITIAL_ALTITUDE=0, DISTANCE=2.6, AVERAGE_SLOPE=6.7, CATEGORY="3";</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A60, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=59, STAGE_NUMBER=18, STARTING_AT_KM=56, NAME="Côte de Loucrup", INITIAL_ALTITUDE=0, DISTANCE=2, AVERAGE_SLOPE=7;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=59, STAGE_NUMBER=18, STARTING_AT_KM=56, NAME="Côte de Loucrup", INITIAL_ALTITUDE=0, DISTANCE=2, AVERAGE_SLOPE=7, CATEGORY="3";</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A61, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=60, STAGE_NUMBER=18, STARTING_AT_KM=95.5, NAME="Col du Tourmalet - Souvenir Jacques Goddet", INITIAL_ALTITUDE=2115, DISTANCE=17.1, AVERAGE_SLOPE=7.3;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=60, STAGE_NUMBER=18, STARTING_AT_KM=95.5, NAME="Col du Tourmalet - Souvenir Jacques Goddet", INITIAL_ALTITUDE=2115, DISTANCE=17.1, AVERAGE_SLOPE=7.3, CATEGORY="H";</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A62, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=61, STAGE_NUMBER=18, STARTING_AT_KM=145.5, NAME="Montée du Hautacam", INITIAL_ALTITUDE=1520, DISTANCE=13.6, AVERAGE_SLOPE=7.8;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=61, STAGE_NUMBER=18, STARTING_AT_KM=145.5, NAME="Montée du Hautacam", INITIAL_ALTITUDE=1520, DISTANCE=13.6, AVERAGE_SLOPE=7.8, CATEGORY="H";</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A63, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=62, STAGE_NUMBER=19, STARTING_AT_KM=195.5, NAME="Côte de Monbazillac", INITIAL_ALTITUDE=0, DISTANCE=1.3, AVERAGE_SLOPE=7.6;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=62, STAGE_NUMBER=19, STARTING_AT_KM=195.5, NAME="Côte de Monbazillac", INITIAL_ALTITUDE=0, DISTANCE=1.3, AVERAGE_SLOPE=7.6, CATEGORY="4";</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
         <f>CONCATENATE("CREATE VERTEX Climb SET ", 'concat fields &amp; values'!A64, ";")</f>
-        <v>CREATE VERTEX Climb SET CLIMB_ID=63, STAGE_NUMBER=21, STARTING_AT_KM=31, NAME="Côte de Briis-sous-Forges", INITIAL_ALTITUDE=0, DISTANCE=0, AVERAGE_SLOPE=0;</v>
+        <v>CREATE VERTEX Climb SET CLIMB_ID=63, STAGE_NUMBER=21, STARTING_AT_KM=31, NAME="Côte de Briis-sous-Forges", INITIAL_ALTITUDE=0, DISTANCE=0, AVERAGE_SLOPE=0, CATEGORY="4";</v>
       </c>
     </row>
   </sheetData>

</xml_diff>